<commit_message>
fix lỗi. Còn phần "đối tác", p chỉnh lại cho nó ngay tí, th chỉnh css của P sợ nó lại bị đụng lung tung nha.
</commit_message>
<xml_diff>
--- a/buylink.nover.vn_v2_fix.xlsx
+++ b/buylink.nover.vn_v2_fix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="120">
   <si>
     <t>Chuyên Mục</t>
   </si>
@@ -718,6 +718,15 @@
   </si>
   <si>
     <t>Đã fix theo như thiết kế</t>
+  </si>
+  <si>
+    <t>Thiết kế như vậy, không thấy tiếng việt</t>
+  </si>
+  <si>
+    <t>link tới register</t>
+  </si>
+  <si>
+    <t>đã fix: theo thiết kế thì đây là nút share.</t>
   </si>
 </sst>
 </file>
@@ -1836,11 +1845,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EX139"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E17" sqref="E17"/>
+      <selection pane="bottomRight" activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3218,7 +3227,9 @@
       <c r="D16" s="144" t="s">
         <v>75</v>
       </c>
-      <c r="E16" s="142"/>
+      <c r="E16" s="142" t="s">
+        <v>115</v>
+      </c>
       <c r="F16" s="142"/>
       <c r="G16" s="142"/>
       <c r="H16" s="142"/>
@@ -3379,7 +3390,9 @@
       <c r="D17" s="144" t="s">
         <v>73</v>
       </c>
-      <c r="E17" s="142"/>
+      <c r="E17" s="142" t="s">
+        <v>117</v>
+      </c>
       <c r="F17" s="142"/>
       <c r="G17" s="142"/>
       <c r="H17" s="142"/>
@@ -3540,7 +3553,9 @@
       <c r="D18" s="145" t="s">
         <v>77</v>
       </c>
-      <c r="E18" s="37"/>
+      <c r="E18" s="37" t="s">
+        <v>115</v>
+      </c>
       <c r="F18" s="37"/>
       <c r="G18" s="37"/>
       <c r="H18" s="37"/>
@@ -4192,7 +4207,9 @@
       <c r="D23" s="93" t="s">
         <v>14</v>
       </c>
-      <c r="E23" s="27"/>
+      <c r="E23" s="27" t="s">
+        <v>113</v>
+      </c>
       <c r="F23" s="27"/>
       <c r="G23" s="27"/>
       <c r="H23" s="27"/>
@@ -5013,7 +5030,9 @@
       <c r="D30" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="E30" s="11"/>
+      <c r="E30" s="11" t="s">
+        <v>118</v>
+      </c>
       <c r="F30" s="11"/>
       <c r="G30" s="11"/>
       <c r="H30" s="11"/>
@@ -5173,6 +5192,9 @@
       </c>
       <c r="D31" s="82" t="s">
         <v>33</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="32" spans="1:153" ht="15.75" x14ac:dyDescent="0.25">
@@ -5361,6 +5383,9 @@
       <c r="D35" s="82" t="s">
         <v>92</v>
       </c>
+      <c r="E35" s="11" t="s">
+        <v>113</v>
+      </c>
     </row>
     <row r="36" spans="1:153" s="4" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="158" t="s">
@@ -5532,7 +5557,9 @@
       <c r="D37" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="E37" s="11"/>
+      <c r="E37" s="11" t="s">
+        <v>113</v>
+      </c>
       <c r="F37" s="11"/>
       <c r="G37" s="11"/>
       <c r="H37" s="11"/>
@@ -5850,7 +5877,9 @@
       <c r="D39" s="131" t="s">
         <v>87</v>
       </c>
-      <c r="E39" s="124"/>
+      <c r="E39" s="124" t="s">
+        <v>113</v>
+      </c>
       <c r="F39" s="124"/>
       <c r="G39" s="124"/>
       <c r="H39" s="124"/>
@@ -6179,6 +6208,9 @@
       </c>
       <c r="D42" s="93" t="s">
         <v>33</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="43" spans="1:153" s="69" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">

</xml_diff>